<commit_message>
Update data and try fix prediction off-trade
</commit_message>
<xml_diff>
--- a/pred_results/on-trade_all_pred_result.xlsx
+++ b/pred_results/on-trade_all_pred_result.xlsx
@@ -580,7 +580,7 @@
         <v>2946</v>
       </c>
       <c r="R2" t="n">
-        <v>3007</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="3">
@@ -638,7 +638,7 @@
         <v>455</v>
       </c>
       <c r="R3" t="n">
-        <v>474</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4">
@@ -696,7 +696,7 @@
         <v>854</v>
       </c>
       <c r="R4" t="n">
-        <v>1209</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="5">
@@ -754,7 +754,7 @@
         <v>118.8125</v>
       </c>
       <c r="R5" t="n">
-        <v>158</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6">
@@ -812,7 +812,7 @@
         <v>3836</v>
       </c>
       <c r="R6" t="n">
-        <v>4352</v>
+        <v>4201</v>
       </c>
     </row>
     <row r="7">
@@ -870,7 +870,7 @@
         <v>716</v>
       </c>
       <c r="R7" t="n">
-        <v>845</v>
+        <v>841</v>
       </c>
     </row>
     <row r="8">
@@ -928,7 +928,7 @@
         <v>11256</v>
       </c>
       <c r="R8" t="n">
-        <v>11437</v>
+        <v>10873</v>
       </c>
     </row>
     <row r="9">
@@ -986,7 +986,7 @@
         <v>1557</v>
       </c>
       <c r="R9" t="n">
-        <v>1934</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="10">
@@ -1044,7 +1044,7 @@
         <v>189.25</v>
       </c>
       <c r="R10" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11">
@@ -1102,7 +1102,7 @@
         <v>536</v>
       </c>
       <c r="R11" t="n">
-        <v>297</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12">
@@ -1154,7 +1154,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="n">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -1212,7 +1212,7 @@
         <v>499</v>
       </c>
       <c r="R13" t="n">
-        <v>422</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14">
@@ -1270,7 +1270,7 @@
         <v>3128</v>
       </c>
       <c r="R14" t="n">
-        <v>2453</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="15">
@@ -1328,7 +1328,7 @@
         <v>391</v>
       </c>
       <c r="R15" t="n">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16">
@@ -1386,7 +1386,7 @@
         <v>170.375</v>
       </c>
       <c r="R16" t="n">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17">
@@ -1444,7 +1444,7 @@
         <v>37.8125</v>
       </c>
       <c r="R17" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
@@ -1502,7 +1502,7 @@
         <v>1326</v>
       </c>
       <c r="R18" t="n">
-        <v>998</v>
+        <v>925</v>
       </c>
     </row>
     <row r="19">
@@ -1560,7 +1560,7 @@
         <v>1115</v>
       </c>
       <c r="R19" t="n">
-        <v>903</v>
+        <v>885</v>
       </c>
     </row>
     <row r="20">
@@ -1618,7 +1618,7 @@
         <v>205</v>
       </c>
       <c r="R20" t="n">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21">
@@ -1676,7 +1676,7 @@
         <v>762</v>
       </c>
       <c r="R21" t="n">
-        <v>833</v>
+        <v>777</v>
       </c>
     </row>
     <row r="22">
@@ -1734,7 +1734,7 @@
         <v>168.25</v>
       </c>
       <c r="R22" t="n">
-        <v>173</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23">
@@ -1792,7 +1792,7 @@
         <v>9488</v>
       </c>
       <c r="R23" t="n">
-        <v>6026</v>
+        <v>5940</v>
       </c>
     </row>
     <row r="24">
@@ -1850,7 +1850,7 @@
         <v>1256</v>
       </c>
       <c r="R24" t="n">
-        <v>1123</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="25">
@@ -1908,7 +1908,7 @@
         <v>260</v>
       </c>
       <c r="R25" t="n">
-        <v>184</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
@@ -1966,7 +1966,7 @@
         <v>84.875</v>
       </c>
       <c r="R26" t="n">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27">
@@ -2024,7 +2024,7 @@
         <v>1058</v>
       </c>
       <c r="R27" t="n">
-        <v>483</v>
+        <v>456</v>
       </c>
     </row>
     <row r="28">
@@ -2082,7 +2082,7 @@
         <v>207</v>
       </c>
       <c r="R28" t="n">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29">
@@ -2134,7 +2134,7 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30">
@@ -2192,7 +2192,7 @@
         <v>121.1875</v>
       </c>
       <c r="R30" t="n">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31">
@@ -2250,7 +2250,7 @@
         <v>1298</v>
       </c>
       <c r="R31" t="n">
-        <v>1122</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="32">
@@ -2308,7 +2308,7 @@
         <v>151.25</v>
       </c>
       <c r="R32" t="n">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33">
@@ -2366,7 +2366,7 @@
         <v>1136</v>
       </c>
       <c r="R33" t="n">
-        <v>835</v>
+        <v>746</v>
       </c>
     </row>
     <row r="34">
@@ -2424,7 +2424,7 @@
         <v>59.6875</v>
       </c>
       <c r="R34" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35">
@@ -2474,7 +2474,7 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
@@ -2528,7 +2528,7 @@
         <v>25.5</v>
       </c>
       <c r="R36" t="n">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37">
@@ -2586,7 +2586,7 @@
         <v>1191</v>
       </c>
       <c r="R37" t="n">
-        <v>1030</v>
+        <v>986</v>
       </c>
     </row>
     <row r="38">
@@ -2644,7 +2644,7 @@
         <v>25</v>
       </c>
       <c r="R38" t="n">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39">
@@ -2702,7 +2702,7 @@
         <v>288.25</v>
       </c>
       <c r="R39" t="n">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="40">
@@ -2754,7 +2754,7 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41">
@@ -2812,7 +2812,7 @@
         <v>930</v>
       </c>
       <c r="R41" t="n">
-        <v>1217</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="42">
@@ -2870,7 +2870,7 @@
         <v>68.125</v>
       </c>
       <c r="R42" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43">
@@ -2928,7 +2928,7 @@
         <v>5876</v>
       </c>
       <c r="R43" t="n">
-        <v>5988</v>
+        <v>5679</v>
       </c>
     </row>
     <row r="44">
@@ -2986,7 +2986,7 @@
         <v>659.5</v>
       </c>
       <c r="R44" t="n">
-        <v>642</v>
+        <v>624</v>
       </c>
     </row>
     <row r="45">
@@ -3044,7 +3044,7 @@
         <v>316.5</v>
       </c>
       <c r="R45" t="n">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="46">
@@ -3102,7 +3102,7 @@
         <v>95</v>
       </c>
       <c r="R46" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47">
@@ -3160,7 +3160,7 @@
         <v>1055</v>
       </c>
       <c r="R47" t="n">
-        <v>1339</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="48">
@@ -3218,7 +3218,7 @@
         <v>102.3125</v>
       </c>
       <c r="R48" t="n">
-        <v>123</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49">
@@ -3276,7 +3276,7 @@
         <v>9376</v>
       </c>
       <c r="R49" t="n">
-        <v>8191</v>
+        <v>7280</v>
       </c>
     </row>
     <row r="50">
@@ -3334,7 +3334,7 @@
         <v>1728</v>
       </c>
       <c r="R50" t="n">
-        <v>1688</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="51">
@@ -3392,7 +3392,7 @@
         <v>131.5</v>
       </c>
       <c r="R51" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52">
@@ -3450,7 +3450,7 @@
         <v>25.046875</v>
       </c>
       <c r="R52" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53">
@@ -3508,7 +3508,7 @@
         <v>816.5</v>
       </c>
       <c r="R53" t="n">
-        <v>626</v>
+        <v>549</v>
       </c>
     </row>
     <row r="54">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="n">
-        <v>398</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56">
@@ -3674,7 +3674,7 @@
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="n">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57">
@@ -3732,7 +3732,7 @@
         <v>23.703125</v>
       </c>
       <c r="R57" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58">
@@ -3790,7 +3790,7 @@
         <v>165</v>
       </c>
       <c r="R58" t="n">
-        <v>129</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59">
@@ -3842,7 +3842,7 @@
         <v>11</v>
       </c>
       <c r="R59" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60">
@@ -3896,7 +3896,7 @@
         <v>56.375</v>
       </c>
       <c r="R60" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61">
@@ -3954,7 +3954,7 @@
         <v>322.75</v>
       </c>
       <c r="R61" t="n">
-        <v>282</v>
+        <v>220</v>
       </c>
     </row>
     <row r="62">
@@ -4012,7 +4012,7 @@
         <v>63.3125</v>
       </c>
       <c r="R62" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63">
@@ -4070,7 +4070,7 @@
         <v>1932</v>
       </c>
       <c r="R63" t="n">
-        <v>1360</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="64">
@@ -4128,7 +4128,7 @@
         <v>425.5</v>
       </c>
       <c r="R64" t="n">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
     <row r="65">
@@ -4186,7 +4186,7 @@
         <v>64.9375</v>
       </c>
       <c r="R65" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66">
@@ -4244,7 +4244,7 @@
         <v>664</v>
       </c>
       <c r="R66" t="n">
-        <v>416</v>
+        <v>399</v>
       </c>
     </row>
     <row r="67">
@@ -4302,7 +4302,7 @@
         <v>36</v>
       </c>
       <c r="R67" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68">
@@ -4360,7 +4360,7 @@
         <v>841.5</v>
       </c>
       <c r="R68" t="n">
-        <v>779</v>
+        <v>706</v>
       </c>
     </row>
     <row r="69">
@@ -4418,7 +4418,7 @@
         <v>75</v>
       </c>
       <c r="R69" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70">
@@ -4470,7 +4470,7 @@
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="n">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71">
@@ -4528,7 +4528,7 @@
         <v>1078</v>
       </c>
       <c r="R71" t="n">
-        <v>1456</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="72">
@@ -4586,7 +4586,7 @@
         <v>45.90625</v>
       </c>
       <c r="R72" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73">
@@ -4644,7 +4644,7 @@
         <v>10472</v>
       </c>
       <c r="R73" t="n">
-        <v>8901</v>
+        <v>8423</v>
       </c>
     </row>
     <row r="74">
@@ -4702,7 +4702,7 @@
         <v>444.5</v>
       </c>
       <c r="R74" t="n">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75">
@@ -4760,7 +4760,7 @@
         <v>363</v>
       </c>
       <c r="R75" t="n">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76">
@@ -4818,7 +4818,7 @@
         <v>123.5</v>
       </c>
       <c r="R76" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77">
@@ -4876,7 +4876,7 @@
         <v>299</v>
       </c>
       <c r="R77" t="n">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78">
@@ -4934,7 +4934,7 @@
         <v>67.8125</v>
       </c>
       <c r="R78" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79">
@@ -4992,7 +4992,7 @@
         <v>37.0625</v>
       </c>
       <c r="R79" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80">
@@ -5050,7 +5050,7 @@
         <v>25.796875</v>
       </c>
       <c r="R80" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81">
@@ -5108,7 +5108,7 @@
         <v>20.40625</v>
       </c>
       <c r="R81" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82">
@@ -5158,7 +5158,7 @@
       <c r="P82" t="inlineStr"/>
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83">
@@ -5216,7 +5216,7 @@
         <v>159.75</v>
       </c>
       <c r="R83" t="n">
-        <v>224</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84">
@@ -5274,7 +5274,7 @@
         <v>56.40625</v>
       </c>
       <c r="R84" t="n">
-        <v>134</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85">
@@ -5332,7 +5332,7 @@
         <v>1852</v>
       </c>
       <c r="R85" t="n">
-        <v>2226</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="86">
@@ -5390,7 +5390,7 @@
         <v>1114</v>
       </c>
       <c r="R86" t="n">
-        <v>796</v>
+        <v>730</v>
       </c>
     </row>
     <row r="87">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="Q87" t="inlineStr"/>
       <c r="R87" t="n">
-        <v>445</v>
+        <v>513</v>
       </c>
     </row>
     <row r="88">
@@ -5502,7 +5502,7 @@
         <v>233</v>
       </c>
       <c r="R88" t="n">
-        <v>245</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89">
@@ -5560,7 +5560,7 @@
         <v>68.0625</v>
       </c>
       <c r="R89" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90">
@@ -5618,7 +5618,7 @@
         <v>214.25</v>
       </c>
       <c r="R90" t="n">
-        <v>187</v>
+        <v>148</v>
       </c>
     </row>
     <row r="91">
@@ -5668,7 +5668,7 @@
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="inlineStr"/>
       <c r="R91" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92">
@@ -5726,7 +5726,7 @@
         <v>299</v>
       </c>
       <c r="R92" t="n">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93">
@@ -5784,7 +5784,7 @@
         <v>878</v>
       </c>
       <c r="R93" t="n">
-        <v>759</v>
+        <v>677</v>
       </c>
     </row>
     <row r="94">
@@ -5842,7 +5842,7 @@
         <v>727.5</v>
       </c>
       <c r="R94" t="n">
-        <v>543</v>
+        <v>514</v>
       </c>
     </row>
     <row r="95">
@@ -5900,7 +5900,7 @@
         <v>3430</v>
       </c>
       <c r="R95" t="n">
-        <v>2187</v>
+        <v>2818</v>
       </c>
     </row>
     <row r="96">
@@ -5956,7 +5956,7 @@
         <v>410</v>
       </c>
       <c r="R96" t="n">
-        <v>555</v>
+        <v>502</v>
       </c>
     </row>
     <row r="97">
@@ -6014,7 +6014,7 @@
         <v>981</v>
       </c>
       <c r="R97" t="n">
-        <v>983</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="98">
@@ -6072,7 +6072,7 @@
         <v>107.6875</v>
       </c>
       <c r="R98" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="99">
@@ -6130,7 +6130,7 @@
         <v>3356</v>
       </c>
       <c r="R99" t="n">
-        <v>3297</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="100">
@@ -6188,7 +6188,7 @@
         <v>738.5</v>
       </c>
       <c r="R100" t="n">
-        <v>656</v>
+        <v>673</v>
       </c>
     </row>
     <row r="101">
@@ -6246,7 +6246,7 @@
         <v>14304</v>
       </c>
       <c r="R101" t="n">
-        <v>10519</v>
+        <v>12466</v>
       </c>
     </row>
     <row r="102">
@@ -6304,7 +6304,7 @@
         <v>1686</v>
       </c>
       <c r="R102" t="n">
-        <v>1454</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="103">
@@ -6362,7 +6362,7 @@
         <v>127.5</v>
       </c>
       <c r="R103" t="n">
-        <v>116</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104">
@@ -6420,7 +6420,7 @@
         <v>403.5</v>
       </c>
       <c r="R104" t="n">
-        <v>220</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105">
@@ -6472,7 +6472,7 @@
       <c r="P105" t="inlineStr"/>
       <c r="Q105" t="inlineStr"/>
       <c r="R105" t="n">
-        <v>56</v>
+        <v>84</v>
       </c>
     </row>
     <row r="106">
@@ -6530,7 +6530,7 @@
         <v>513</v>
       </c>
       <c r="R106" t="n">
-        <v>313</v>
+        <v>387</v>
       </c>
     </row>
     <row r="107">
@@ -6588,7 +6588,7 @@
         <v>3438</v>
       </c>
       <c r="R107" t="n">
-        <v>1849</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="108">
@@ -6646,7 +6646,7 @@
         <v>361.5</v>
       </c>
       <c r="R108" t="n">
-        <v>198</v>
+        <v>265</v>
       </c>
     </row>
     <row r="109">
@@ -6704,7 +6704,7 @@
         <v>157.75</v>
       </c>
       <c r="R109" t="n">
-        <v>95</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110">
@@ -6762,7 +6762,7 @@
         <v>31.21875</v>
       </c>
       <c r="R110" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="111">
@@ -6820,7 +6820,7 @@
         <v>1794</v>
       </c>
       <c r="R111" t="n">
-        <v>769</v>
+        <v>856</v>
       </c>
     </row>
     <row r="112">
@@ -6878,7 +6878,7 @@
         <v>1328</v>
       </c>
       <c r="R112" t="n">
-        <v>776</v>
+        <v>926</v>
       </c>
     </row>
     <row r="113">
@@ -6936,7 +6936,7 @@
         <v>155</v>
       </c>
       <c r="R113" t="n">
-        <v>107</v>
+        <v>135</v>
       </c>
     </row>
     <row r="114">
@@ -6994,7 +6994,7 @@
         <v>972</v>
       </c>
       <c r="R114" t="n">
-        <v>658</v>
+        <v>694</v>
       </c>
     </row>
     <row r="115">
@@ -7052,7 +7052,7 @@
         <v>129.25</v>
       </c>
       <c r="R115" t="n">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="116">
@@ -7110,7 +7110,7 @@
         <v>10752</v>
       </c>
       <c r="R116" t="n">
-        <v>5121</v>
+        <v>7890</v>
       </c>
     </row>
     <row r="117">
@@ -7168,7 +7168,7 @@
         <v>1410</v>
       </c>
       <c r="R117" t="n">
-        <v>816</v>
+        <v>904</v>
       </c>
     </row>
     <row r="118">
@@ -7226,7 +7226,7 @@
         <v>335.5</v>
       </c>
       <c r="R118" t="n">
-        <v>148</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119">
@@ -7284,7 +7284,7 @@
         <v>57.59375</v>
       </c>
       <c r="R119" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="120">
@@ -7342,7 +7342,7 @@
         <v>1514</v>
       </c>
       <c r="R120" t="n">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="121">
@@ -7398,7 +7398,7 @@
         <v>260.5</v>
       </c>
       <c r="R121" t="n">
-        <v>354</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122">
@@ -7450,7 +7450,7 @@
       <c r="P122" t="inlineStr"/>
       <c r="Q122" t="inlineStr"/>
       <c r="R122" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123">
@@ -7508,7 +7508,7 @@
         <v>117.3125</v>
       </c>
       <c r="R123" t="n">
-        <v>101</v>
+        <v>129</v>
       </c>
     </row>
     <row r="124">
@@ -7566,7 +7566,7 @@
         <v>1520</v>
       </c>
       <c r="R124" t="n">
-        <v>810</v>
+        <v>938</v>
       </c>
     </row>
     <row r="125">
@@ -7624,7 +7624,7 @@
         <v>177.25</v>
       </c>
       <c r="R125" t="n">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="126">
@@ -7682,7 +7682,7 @@
         <v>1208</v>
       </c>
       <c r="R126" t="n">
-        <v>640</v>
+        <v>682</v>
       </c>
     </row>
     <row r="127">
@@ -7740,7 +7740,7 @@
         <v>73.1875</v>
       </c>
       <c r="R127" t="n">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="128">
@@ -7792,7 +7792,7 @@
       </c>
       <c r="Q128" t="inlineStr"/>
       <c r="R128" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129">
@@ -7846,7 +7846,7 @@
         <v>54</v>
       </c>
       <c r="R129" t="n">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130">
@@ -7904,7 +7904,7 @@
         <v>1102</v>
       </c>
       <c r="R130" t="n">
-        <v>826</v>
+        <v>856</v>
       </c>
     </row>
     <row r="131">
@@ -7962,7 +7962,7 @@
         <v>10</v>
       </c>
       <c r="R131" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="132">
@@ -8020,7 +8020,7 @@
         <v>292</v>
       </c>
       <c r="R132" t="n">
-        <v>454</v>
+        <v>406</v>
       </c>
     </row>
     <row r="133">
@@ -8072,7 +8072,7 @@
       <c r="P133" t="inlineStr"/>
       <c r="Q133" t="inlineStr"/>
       <c r="R133" t="n">
-        <v>32</v>
+        <v>62</v>
       </c>
     </row>
     <row r="134">
@@ -8130,7 +8130,7 @@
         <v>752.5</v>
       </c>
       <c r="R134" t="n">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
     <row r="135">
@@ -8188,7 +8188,7 @@
         <v>62.40625</v>
       </c>
       <c r="R135" t="n">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="136">
@@ -8246,7 +8246,7 @@
         <v>5468</v>
       </c>
       <c r="R136" t="n">
-        <v>4893</v>
+        <v>5653</v>
       </c>
     </row>
     <row r="137">
@@ -8304,7 +8304,7 @@
         <v>627.5</v>
       </c>
       <c r="R137" t="n">
-        <v>450</v>
+        <v>504</v>
       </c>
     </row>
     <row r="138">
@@ -8362,7 +8362,7 @@
         <v>389</v>
       </c>
       <c r="R138" t="n">
-        <v>262</v>
+        <v>307</v>
       </c>
     </row>
     <row r="139">
@@ -8420,7 +8420,7 @@
         <v>90</v>
       </c>
       <c r="R139" t="n">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="140">
@@ -8478,7 +8478,7 @@
         <v>869.5</v>
       </c>
       <c r="R140" t="n">
-        <v>1098</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="141">
@@ -8536,7 +8536,7 @@
         <v>113.125</v>
       </c>
       <c r="R141" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142">
@@ -8594,7 +8594,7 @@
         <v>8392</v>
       </c>
       <c r="R142" t="n">
-        <v>6447</v>
+        <v>7927</v>
       </c>
     </row>
     <row r="143">
@@ -8652,7 +8652,7 @@
         <v>2276</v>
       </c>
       <c r="R143" t="n">
-        <v>1417</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="144">
@@ -8710,7 +8710,7 @@
         <v>139.25</v>
       </c>
       <c r="R144" t="n">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="145">
@@ -8768,7 +8768,7 @@
         <v>37.9375</v>
       </c>
       <c r="R145" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="146">
@@ -8826,7 +8826,7 @@
         <v>950.5</v>
       </c>
       <c r="R146" t="n">
-        <v>463</v>
+        <v>510</v>
       </c>
     </row>
     <row r="147">
@@ -8884,7 +8884,7 @@
         <v>113.125</v>
       </c>
       <c r="R147" t="n">
-        <v>74</v>
+        <v>82</v>
       </c>
     </row>
     <row r="148">
@@ -8940,7 +8940,7 @@
       </c>
       <c r="Q148" t="inlineStr"/>
       <c r="R148" t="n">
-        <v>311</v>
+        <v>359</v>
       </c>
     </row>
     <row r="149">
@@ -8992,7 +8992,7 @@
       <c r="P149" t="inlineStr"/>
       <c r="Q149" t="inlineStr"/>
       <c r="R149" t="n">
-        <v>121</v>
+        <v>151</v>
       </c>
     </row>
     <row r="150">
@@ -9050,7 +9050,7 @@
         <v>26.09375</v>
       </c>
       <c r="R150" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="151">
@@ -9108,7 +9108,7 @@
         <v>174</v>
       </c>
       <c r="R151" t="n">
-        <v>112</v>
+        <v>170</v>
       </c>
     </row>
     <row r="152">
@@ -9160,7 +9160,7 @@
         <v>11.5</v>
       </c>
       <c r="R152" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="153">
@@ -9214,7 +9214,7 @@
         <v>84.9375</v>
       </c>
       <c r="R153" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="154">
@@ -9272,7 +9272,7 @@
         <v>340</v>
       </c>
       <c r="R154" t="n">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="155">
@@ -9330,7 +9330,7 @@
         <v>47.6875</v>
       </c>
       <c r="R155" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="156">
@@ -9388,7 +9388,7 @@
         <v>2116</v>
       </c>
       <c r="R156" t="n">
-        <v>1026</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="157">
@@ -9446,7 +9446,7 @@
         <v>451</v>
       </c>
       <c r="R157" t="n">
-        <v>199</v>
+        <v>226</v>
       </c>
     </row>
     <row r="158">
@@ -9504,7 +9504,7 @@
         <v>72.75</v>
       </c>
       <c r="R158" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="159">
@@ -9562,7 +9562,7 @@
         <v>725</v>
       </c>
       <c r="R159" t="n">
-        <v>323</v>
+        <v>343</v>
       </c>
     </row>
     <row r="160">
@@ -9620,7 +9620,7 @@
         <v>38</v>
       </c>
       <c r="R160" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="161">
@@ -9678,7 +9678,7 @@
         <v>979.5</v>
       </c>
       <c r="R161" t="n">
-        <v>536</v>
+        <v>573</v>
       </c>
     </row>
     <row r="162">
@@ -9734,7 +9734,7 @@
         <v>60</v>
       </c>
       <c r="R162" t="n">
-        <v>112</v>
+        <v>57</v>
       </c>
     </row>
     <row r="163">
@@ -9786,7 +9786,7 @@
       <c r="P163" t="inlineStr"/>
       <c r="Q163" t="inlineStr"/>
       <c r="R163" t="n">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="164">
@@ -9844,7 +9844,7 @@
         <v>1140</v>
       </c>
       <c r="R164" t="n">
-        <v>1053</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="165">
@@ -9902,7 +9902,7 @@
         <v>41.6875</v>
       </c>
       <c r="R165" t="n">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="166">
@@ -9960,7 +9960,7 @@
         <v>11152</v>
       </c>
       <c r="R166" t="n">
-        <v>7129</v>
+        <v>8977</v>
       </c>
     </row>
     <row r="167">
@@ -10018,7 +10018,7 @@
         <v>448.5</v>
       </c>
       <c r="R167" t="n">
-        <v>204</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168">
@@ -10076,7 +10076,7 @@
         <v>483</v>
       </c>
       <c r="R168" t="n">
-        <v>194</v>
+        <v>240</v>
       </c>
     </row>
     <row r="169">
@@ -10134,7 +10134,7 @@
         <v>133</v>
       </c>
       <c r="R169" t="n">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="170">
@@ -10192,7 +10192,7 @@
         <v>274</v>
       </c>
       <c r="R170" t="n">
-        <v>116</v>
+        <v>161</v>
       </c>
     </row>
     <row r="171">
@@ -10250,7 +10250,7 @@
         <v>73.8125</v>
       </c>
       <c r="R171" t="n">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="172">
@@ -10308,7 +10308,7 @@
         <v>36.90625</v>
       </c>
       <c r="R172" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="173">
@@ -10366,7 +10366,7 @@
         <v>25.5</v>
       </c>
       <c r="R173" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="174">
@@ -10424,7 +10424,7 @@
         <v>18.59375</v>
       </c>
       <c r="R174" t="n">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="175">
@@ -10474,7 +10474,7 @@
       <c r="P175" t="inlineStr"/>
       <c r="Q175" t="inlineStr"/>
       <c r="R175" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="176">
@@ -10532,7 +10532,7 @@
         <v>164.875</v>
       </c>
       <c r="R176" t="n">
-        <v>176</v>
+        <v>185</v>
       </c>
     </row>
     <row r="177">
@@ -10590,7 +10590,7 @@
         <v>61.9375</v>
       </c>
       <c r="R177" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="178">
@@ -10648,7 +10648,7 @@
         <v>2232</v>
       </c>
       <c r="R178" t="n">
-        <v>1741</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="179">
@@ -10706,7 +10706,7 @@
         <v>956.5</v>
       </c>
       <c r="R179" t="n">
-        <v>626</v>
+        <v>696</v>
       </c>
     </row>
     <row r="180">
@@ -10760,7 +10760,7 @@
       </c>
       <c r="Q180" t="inlineStr"/>
       <c r="R180" t="n">
-        <v>462</v>
+        <v>411</v>
       </c>
     </row>
     <row r="181">
@@ -10818,7 +10818,7 @@
         <v>378.75</v>
       </c>
       <c r="R181" t="n">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="182">
@@ -10876,7 +10876,7 @@
         <v>71.125</v>
       </c>
       <c r="R182" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="183">
@@ -10934,7 +10934,7 @@
         <v>356</v>
       </c>
       <c r="R183" t="n">
-        <v>181</v>
+        <v>205</v>
       </c>
     </row>
     <row r="184">
@@ -10986,7 +10986,7 @@
         <v>17.4375</v>
       </c>
       <c r="R184" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="185">
@@ -11044,7 +11044,7 @@
         <v>259</v>
       </c>
       <c r="R185" t="n">
-        <v>173</v>
+        <v>205</v>
       </c>
     </row>
     <row r="186">
@@ -11102,7 +11102,7 @@
         <v>925.5</v>
       </c>
       <c r="R186" t="n">
-        <v>560</v>
+        <v>624</v>
       </c>
     </row>
     <row r="187">
@@ -11160,7 +11160,7 @@
         <v>607</v>
       </c>
       <c r="R187" t="n">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="188">
@@ -11216,7 +11216,7 @@
         <v>2494</v>
       </c>
       <c r="R188" t="n">
-        <v>1200</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="189">
@@ -11270,7 +11270,7 @@
         <v>420</v>
       </c>
       <c r="R189" t="n">
-        <v>410</v>
+        <v>599</v>
       </c>
     </row>
     <row r="190">
@@ -11326,7 +11326,7 @@
         <v>908</v>
       </c>
       <c r="R190" t="n">
-        <v>543</v>
+        <v>701</v>
       </c>
     </row>
     <row r="191">
@@ -11382,7 +11382,7 @@
         <v>101.375</v>
       </c>
       <c r="R191" t="n">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="192">
@@ -11438,7 +11438,7 @@
         <v>1750</v>
       </c>
       <c r="R192" t="n">
-        <v>1138</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="193">
@@ -11494,7 +11494,7 @@
         <v>621.5</v>
       </c>
       <c r="R193" t="n">
-        <v>459</v>
+        <v>546</v>
       </c>
     </row>
     <row r="194">
@@ -11550,7 +11550,7 @@
         <v>11216</v>
       </c>
       <c r="R194" t="n">
-        <v>2950</v>
+        <v>10014</v>
       </c>
     </row>
     <row r="195">
@@ -11606,7 +11606,7 @@
         <v>1486</v>
       </c>
       <c r="R195" t="n">
-        <v>909</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="196">
@@ -11662,7 +11662,7 @@
         <v>147.875</v>
       </c>
       <c r="R196" t="n">
-        <v>186</v>
+        <v>142</v>
       </c>
     </row>
     <row r="197">
@@ -11718,7 +11718,7 @@
         <v>337</v>
       </c>
       <c r="R197" t="n">
-        <v>320</v>
+        <v>286</v>
       </c>
     </row>
     <row r="198">
@@ -11768,7 +11768,7 @@
       <c r="P198" t="inlineStr"/>
       <c r="Q198" t="inlineStr"/>
       <c r="R198" t="n">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="199">
@@ -11824,7 +11824,7 @@
         <v>352</v>
       </c>
       <c r="R199" t="n">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="200">
@@ -11880,7 +11880,7 @@
         <v>2130</v>
       </c>
       <c r="R200" t="n">
-        <v>1166</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="201">
@@ -11936,7 +11936,7 @@
         <v>276.5</v>
       </c>
       <c r="R201" t="n">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="202">
@@ -11992,7 +11992,7 @@
         <v>132.25</v>
       </c>
       <c r="R202" t="n">
-        <v>122</v>
+        <v>106</v>
       </c>
     </row>
     <row r="203">
@@ -12048,7 +12048,7 @@
         <v>36.59375</v>
       </c>
       <c r="R203" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="204">
@@ -12104,7 +12104,7 @@
         <v>959</v>
       </c>
       <c r="R204" t="n">
-        <v>494</v>
+        <v>603</v>
       </c>
     </row>
     <row r="205">
@@ -12160,7 +12160,7 @@
         <v>1051</v>
       </c>
       <c r="R205" t="n">
-        <v>496</v>
+        <v>593</v>
       </c>
     </row>
     <row r="206">
@@ -12216,7 +12216,7 @@
         <v>175</v>
       </c>
       <c r="R206" t="n">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="207">
@@ -12272,7 +12272,7 @@
         <v>861.5</v>
       </c>
       <c r="R207" t="n">
-        <v>430</v>
+        <v>469</v>
       </c>
     </row>
     <row r="208">
@@ -12328,7 +12328,7 @@
         <v>192</v>
       </c>
       <c r="R208" t="n">
-        <v>240</v>
+        <v>195</v>
       </c>
     </row>
     <row r="209">
@@ -12384,7 +12384,7 @@
         <v>6328</v>
       </c>
       <c r="R209" t="n">
-        <v>1743</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="210">
@@ -12440,7 +12440,7 @@
         <v>1050</v>
       </c>
       <c r="R210" t="n">
-        <v>602</v>
+        <v>784</v>
       </c>
     </row>
     <row r="211">
@@ -12496,7 +12496,7 @@
         <v>220.25</v>
       </c>
       <c r="R211" t="n">
-        <v>155</v>
+        <v>102</v>
       </c>
     </row>
     <row r="212">
@@ -12552,7 +12552,7 @@
         <v>45</v>
       </c>
       <c r="R212" t="n">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="213">
@@ -12608,7 +12608,7 @@
         <v>1445</v>
       </c>
       <c r="R213" t="n">
-        <v>433</v>
+        <v>477</v>
       </c>
     </row>
     <row r="214">
@@ -12662,7 +12662,7 @@
         <v>219.75</v>
       </c>
       <c r="R214" t="n">
-        <v>44</v>
+        <v>136</v>
       </c>
     </row>
     <row r="215">
@@ -12712,7 +12712,7 @@
       <c r="P215" t="inlineStr"/>
       <c r="Q215" t="inlineStr"/>
       <c r="R215" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216">
@@ -12768,7 +12768,7 @@
         <v>124.1875</v>
       </c>
       <c r="R216" t="n">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="217">
@@ -12824,7 +12824,7 @@
         <v>1272</v>
       </c>
       <c r="R217" t="n">
-        <v>566</v>
+        <v>796</v>
       </c>
     </row>
     <row r="218">
@@ -12880,7 +12880,7 @@
         <v>153.625</v>
       </c>
       <c r="R218" t="n">
-        <v>201</v>
+        <v>158</v>
       </c>
     </row>
     <row r="219">
@@ -12936,7 +12936,7 @@
         <v>1142</v>
       </c>
       <c r="R219" t="n">
-        <v>519</v>
+        <v>642</v>
       </c>
     </row>
     <row r="220">
@@ -12992,7 +12992,7 @@
         <v>80.125</v>
       </c>
       <c r="R220" t="n">
-        <v>44</v>
+        <v>65</v>
       </c>
     </row>
     <row r="221">
@@ -13044,7 +13044,7 @@
       </c>
       <c r="Q221" t="inlineStr"/>
       <c r="R221" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222">
@@ -13098,7 +13098,7 @@
         <v>42.90625</v>
       </c>
       <c r="R222" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="223">
@@ -13154,7 +13154,7 @@
         <v>1116</v>
       </c>
       <c r="R223" t="n">
-        <v>547</v>
+        <v>675</v>
       </c>
     </row>
     <row r="224">
@@ -13210,7 +13210,7 @@
         <v>20</v>
       </c>
       <c r="R224" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="225">
@@ -13266,7 +13266,7 @@
         <v>306</v>
       </c>
       <c r="R225" t="n">
-        <v>387</v>
+        <v>398</v>
       </c>
     </row>
     <row r="226">
@@ -13316,7 +13316,7 @@
       <c r="P226" t="inlineStr"/>
       <c r="Q226" t="inlineStr"/>
       <c r="R226" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="227">
@@ -13372,7 +13372,7 @@
         <v>730</v>
       </c>
       <c r="R227" t="n">
-        <v>560</v>
+        <v>665</v>
       </c>
     </row>
     <row r="228">
@@ -13428,7 +13428,7 @@
         <v>61.5</v>
       </c>
       <c r="R228" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="229">
@@ -13484,7 +13484,7 @@
         <v>5236</v>
       </c>
       <c r="R229" t="n">
-        <v>1390</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="230">
@@ -13540,7 +13540,7 @@
         <v>458.5</v>
       </c>
       <c r="R230" t="n">
-        <v>437</v>
+        <v>481</v>
       </c>
     </row>
     <row r="231">
@@ -13596,7 +13596,7 @@
         <v>393</v>
       </c>
       <c r="R231" t="n">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="232">
@@ -13652,7 +13652,7 @@
         <v>100</v>
       </c>
       <c r="R232" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="233">
@@ -13708,7 +13708,7 @@
         <v>863.5</v>
       </c>
       <c r="R233" t="n">
-        <v>609</v>
+        <v>757</v>
       </c>
     </row>
     <row r="234">
@@ -13764,7 +13764,7 @@
         <v>105.3125</v>
       </c>
       <c r="R234" t="n">
-        <v>149</v>
+        <v>115</v>
       </c>
     </row>
     <row r="235">
@@ -13820,7 +13820,7 @@
         <v>6884</v>
       </c>
       <c r="R235" t="n">
-        <v>2150</v>
+        <v>5981</v>
       </c>
     </row>
     <row r="236">
@@ -13876,7 +13876,7 @@
         <v>1407</v>
       </c>
       <c r="R236" t="n">
-        <v>976</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="237">
@@ -13932,7 +13932,7 @@
         <v>108.4375</v>
       </c>
       <c r="R237" t="n">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="238">
@@ -13988,7 +13988,7 @@
         <v>29.40625</v>
       </c>
       <c r="R238" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="239">
@@ -14044,7 +14044,7 @@
         <v>837.5</v>
       </c>
       <c r="R239" t="n">
-        <v>460</v>
+        <v>467</v>
       </c>
     </row>
     <row r="240">
@@ -14100,7 +14100,7 @@
         <v>98.375</v>
       </c>
       <c r="R240" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="241">
@@ -14154,7 +14154,7 @@
       </c>
       <c r="Q241" t="inlineStr"/>
       <c r="R241" t="n">
-        <v>401</v>
+        <v>426</v>
       </c>
     </row>
     <row r="242">
@@ -14204,7 +14204,7 @@
       <c r="P242" t="inlineStr"/>
       <c r="Q242" t="inlineStr"/>
       <c r="R242" t="n">
-        <v>96</v>
+        <v>139</v>
       </c>
     </row>
     <row r="243">
@@ -14316,7 +14316,7 @@
         <v>144.5</v>
       </c>
       <c r="R244" t="n">
-        <v>251</v>
+        <v>185</v>
       </c>
     </row>
     <row r="245">
@@ -14368,7 +14368,7 @@
         <v>11</v>
       </c>
       <c r="R245" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="246">
@@ -14422,7 +14422,7 @@
         <v>37.84375</v>
       </c>
       <c r="R246" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="247">
@@ -14478,7 +14478,7 @@
         <v>290.75</v>
       </c>
       <c r="R247" t="n">
-        <v>295</v>
+        <v>258</v>
       </c>
     </row>
     <row r="248">
@@ -14590,7 +14590,7 @@
         <v>1834</v>
       </c>
       <c r="R249" t="n">
-        <v>729</v>
+        <v>875</v>
       </c>
     </row>
     <row r="250">
@@ -14646,7 +14646,7 @@
         <v>349</v>
       </c>
       <c r="R250" t="n">
-        <v>327</v>
+        <v>261</v>
       </c>
     </row>
     <row r="251">
@@ -14702,7 +14702,7 @@
         <v>54.59375</v>
       </c>
       <c r="R251" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="252">
@@ -14758,7 +14758,7 @@
         <v>622.5</v>
       </c>
       <c r="R252" t="n">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="253">
@@ -14814,7 +14814,7 @@
         <v>40.5</v>
       </c>
       <c r="R253" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="254">
@@ -14870,7 +14870,7 @@
         <v>867</v>
       </c>
       <c r="R254" t="n">
-        <v>448</v>
+        <v>466</v>
       </c>
     </row>
     <row r="255">
@@ -14924,7 +14924,7 @@
         <v>45</v>
       </c>
       <c r="R255" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="256">
@@ -14974,7 +14974,7 @@
       <c r="P256" t="inlineStr"/>
       <c r="Q256" t="inlineStr"/>
       <c r="R256" t="n">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="257">
@@ -15030,7 +15030,7 @@
         <v>914.5</v>
       </c>
       <c r="R257" t="n">
-        <v>572</v>
+        <v>802</v>
       </c>
     </row>
     <row r="258">
@@ -15086,7 +15086,7 @@
         <v>29.703125</v>
       </c>
       <c r="R258" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="259">
@@ -15142,7 +15142,7 @@
         <v>8456</v>
       </c>
       <c r="R259" t="n">
-        <v>2051</v>
+        <v>7612</v>
       </c>
     </row>
     <row r="260">
@@ -15198,7 +15198,7 @@
         <v>387.5</v>
       </c>
       <c r="R260" t="n">
-        <v>339</v>
+        <v>290</v>
       </c>
     </row>
     <row r="261">
@@ -15254,7 +15254,7 @@
         <v>257</v>
       </c>
       <c r="R261" t="n">
-        <v>303</v>
+        <v>261</v>
       </c>
     </row>
     <row r="262">
@@ -15310,7 +15310,7 @@
         <v>75.5</v>
       </c>
       <c r="R262" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="263">
@@ -15366,7 +15366,7 @@
         <v>209</v>
       </c>
       <c r="R263" t="n">
-        <v>238</v>
+        <v>171</v>
       </c>
     </row>
     <row r="264">
@@ -15422,7 +15422,7 @@
         <v>39.59375</v>
       </c>
       <c r="R264" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="265">
@@ -15478,7 +15478,7 @@
         <v>31.203125</v>
       </c>
       <c r="R265" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="266">
@@ -15534,7 +15534,7 @@
         <v>18.75</v>
       </c>
       <c r="R266" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="267">
@@ -15590,7 +15590,7 @@
         <v>13.796875</v>
       </c>
       <c r="R267" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="268">
@@ -15640,7 +15640,7 @@
       <c r="P268" t="inlineStr"/>
       <c r="Q268" t="inlineStr"/>
       <c r="R268" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="269">
@@ -15696,7 +15696,7 @@
         <v>145.5</v>
       </c>
       <c r="R269" t="n">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="270">
@@ -15752,7 +15752,7 @@
         <v>48.90625</v>
       </c>
       <c r="R270" t="n">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="271">
@@ -15808,7 +15808,7 @@
         <v>1766</v>
       </c>
       <c r="R271" t="n">
-        <v>1180</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="272">
@@ -15864,7 +15864,7 @@
         <v>901.5</v>
       </c>
       <c r="R272" t="n">
-        <v>517</v>
+        <v>601</v>
       </c>
     </row>
     <row r="273">
@@ -15920,7 +15920,7 @@
         <v>175</v>
       </c>
       <c r="R273" t="n">
-        <v>479</v>
+        <v>545</v>
       </c>
     </row>
     <row r="274">
@@ -15976,7 +15976,7 @@
         <v>422</v>
       </c>
       <c r="R274" t="n">
-        <v>381</v>
+        <v>333</v>
       </c>
     </row>
     <row r="275">
@@ -16032,7 +16032,7 @@
         <v>110.1875</v>
       </c>
       <c r="R275" t="n">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="276">
@@ -16088,7 +16088,7 @@
         <v>398</v>
       </c>
       <c r="R276" t="n">
-        <v>307</v>
+        <v>264</v>
       </c>
     </row>
     <row r="277">
@@ -16140,7 +16140,7 @@
         <v>61.34375</v>
       </c>
       <c r="R277" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="278">
@@ -16196,7 +16196,7 @@
         <v>256.5</v>
       </c>
       <c r="R278" t="n">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="279">
@@ -16252,7 +16252,7 @@
         <v>828</v>
       </c>
       <c r="R279" t="n">
-        <v>474</v>
+        <v>494</v>
       </c>
     </row>
     <row r="280">
@@ -16306,7 +16306,7 @@
         <v>688.5</v>
       </c>
       <c r="R280" t="n">
-        <v>371</v>
+        <v>452</v>
       </c>
     </row>
     <row r="281">
@@ -16360,7 +16360,7 @@
         <v>2710</v>
       </c>
       <c r="R281" t="n">
-        <v>1352</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="282">
@@ -16414,7 +16414,7 @@
         <v>395</v>
       </c>
       <c r="R282" t="n">
-        <v>415</v>
+        <v>564</v>
       </c>
     </row>
     <row r="283">
@@ -16468,7 +16468,7 @@
         <v>845.5</v>
       </c>
       <c r="R283" t="n">
-        <v>663</v>
+        <v>774</v>
       </c>
     </row>
     <row r="284">
@@ -16522,7 +16522,7 @@
         <v>106.9375</v>
       </c>
       <c r="R284" t="n">
-        <v>23</v>
+        <v>107</v>
       </c>
     </row>
     <row r="285">
@@ -16576,7 +16576,7 @@
         <v>2782</v>
       </c>
       <c r="R285" t="n">
-        <v>1258</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="286">
@@ -16630,7 +16630,7 @@
         <v>636.5</v>
       </c>
       <c r="R286" t="n">
-        <v>603</v>
+        <v>685</v>
       </c>
     </row>
     <row r="287">
@@ -16684,7 +16684,7 @@
         <v>10072</v>
       </c>
       <c r="R287" t="n">
-        <v>3121</v>
+        <v>9990</v>
       </c>
     </row>
     <row r="288">
@@ -16738,7 +16738,7 @@
         <v>1468</v>
       </c>
       <c r="R288" t="n">
-        <v>982</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="289">
@@ -16792,7 +16792,7 @@
         <v>140.75</v>
       </c>
       <c r="R289" t="n">
-        <v>28</v>
+        <v>90</v>
       </c>
     </row>
     <row r="290">
@@ -16846,7 +16846,7 @@
         <v>355.75</v>
       </c>
       <c r="R290" t="n">
-        <v>224</v>
+        <v>279</v>
       </c>
     </row>
     <row r="291">
@@ -16894,7 +16894,7 @@
       <c r="P291" t="inlineStr"/>
       <c r="Q291" t="inlineStr"/>
       <c r="R291" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="292">
@@ -16948,7 +16948,7 @@
         <v>319.75</v>
       </c>
       <c r="R292" t="n">
-        <v>354</v>
+        <v>431</v>
       </c>
     </row>
     <row r="293">
@@ -17002,7 +17002,7 @@
         <v>2630</v>
       </c>
       <c r="R293" t="n">
-        <v>1384</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="294">
@@ -17056,7 +17056,7 @@
         <v>384.75</v>
       </c>
       <c r="R294" t="n">
-        <v>89</v>
+        <v>215</v>
       </c>
     </row>
     <row r="295">
@@ -17110,7 +17110,7 @@
         <v>121.1875</v>
       </c>
       <c r="R295" t="n">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="296">
@@ -17164,7 +17164,7 @@
         <v>24.90625</v>
       </c>
       <c r="R296" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="297">
@@ -17218,7 +17218,7 @@
         <v>940.5</v>
       </c>
       <c r="R297" t="n">
-        <v>602</v>
+        <v>695</v>
       </c>
     </row>
     <row r="298">
@@ -17272,7 +17272,7 @@
         <v>1122</v>
       </c>
       <c r="R298" t="n">
-        <v>635</v>
+        <v>721</v>
       </c>
     </row>
     <row r="299">
@@ -17326,7 +17326,7 @@
         <v>155</v>
       </c>
       <c r="R299" t="n">
-        <v>15</v>
+        <v>88</v>
       </c>
     </row>
     <row r="300">
@@ -17380,7 +17380,7 @@
         <v>662</v>
       </c>
       <c r="R300" t="n">
-        <v>594</v>
+        <v>612</v>
       </c>
     </row>
     <row r="301">
@@ -17434,7 +17434,7 @@
         <v>182.125</v>
       </c>
       <c r="R301" t="n">
-        <v>32</v>
+        <v>95</v>
       </c>
     </row>
     <row r="302">
@@ -17488,7 +17488,7 @@
         <v>8060</v>
       </c>
       <c r="R302" t="n">
-        <v>2413</v>
+        <v>5730</v>
       </c>
     </row>
     <row r="303">
@@ -17542,7 +17542,7 @@
         <v>1092</v>
       </c>
       <c r="R303" t="n">
-        <v>665</v>
+        <v>833</v>
       </c>
     </row>
     <row r="304">
@@ -17596,7 +17596,7 @@
         <v>214.5</v>
       </c>
       <c r="R304" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="305">
@@ -17650,7 +17650,7 @@
         <v>36.59375</v>
       </c>
       <c r="R305" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="306">
@@ -17704,7 +17704,7 @@
         <v>705</v>
       </c>
       <c r="R306" t="n">
-        <v>251</v>
+        <v>440</v>
       </c>
     </row>
     <row r="307">
@@ -17758,7 +17758,7 @@
         <v>169.75</v>
       </c>
       <c r="R307" t="n">
-        <v>41</v>
+        <v>132</v>
       </c>
     </row>
     <row r="308">
@@ -17806,7 +17806,7 @@
       <c r="P308" t="inlineStr"/>
       <c r="Q308" t="inlineStr"/>
       <c r="R308" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="309">
@@ -17860,7 +17860,7 @@
         <v>95.6875</v>
       </c>
       <c r="R309" t="n">
-        <v>15</v>
+        <v>83</v>
       </c>
     </row>
     <row r="310">
@@ -17914,7 +17914,7 @@
         <v>1218</v>
       </c>
       <c r="R310" t="n">
-        <v>705</v>
+        <v>938</v>
       </c>
     </row>
     <row r="311">
@@ -17968,7 +17968,7 @@
         <v>141</v>
       </c>
       <c r="R311" t="n">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="312">
@@ -18022,7 +18022,7 @@
         <v>1036</v>
       </c>
       <c r="R312" t="n">
-        <v>640</v>
+        <v>781</v>
       </c>
     </row>
     <row r="313">
@@ -18076,7 +18076,7 @@
         <v>70.5</v>
       </c>
       <c r="R313" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="314">
@@ -18128,7 +18128,7 @@
       </c>
       <c r="Q314" t="inlineStr"/>
       <c r="R314" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315">
@@ -18182,7 +18182,7 @@
         <v>22.796875</v>
       </c>
       <c r="R315" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="316">
@@ -18236,7 +18236,7 @@
         <v>1057</v>
       </c>
       <c r="R316" t="n">
-        <v>678</v>
+        <v>808</v>
       </c>
     </row>
     <row r="317">
@@ -18290,7 +18290,7 @@
         <v>15</v>
       </c>
       <c r="R317" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="318">
@@ -18344,7 +18344,7 @@
         <v>267</v>
       </c>
       <c r="R318" t="n">
-        <v>261</v>
+        <v>429</v>
       </c>
     </row>
     <row r="319">
@@ -18392,7 +18392,7 @@
       <c r="P319" t="inlineStr"/>
       <c r="Q319" t="inlineStr"/>
       <c r="R319" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="320">
@@ -18446,7 +18446,7 @@
         <v>711.5</v>
       </c>
       <c r="R320" t="n">
-        <v>646</v>
+        <v>758</v>
       </c>
     </row>
     <row r="321">
@@ -18500,7 +18500,7 @@
         <v>49.8125</v>
       </c>
       <c r="R321" t="n">
-        <v>16</v>
+        <v>56</v>
       </c>
     </row>
     <row r="322">
@@ -18554,7 +18554,7 @@
         <v>4608</v>
       </c>
       <c r="R322" t="n">
-        <v>1794</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="323">
@@ -18608,7 +18608,7 @@
         <v>534</v>
       </c>
       <c r="R323" t="n">
-        <v>547</v>
+        <v>593</v>
       </c>
     </row>
     <row r="324">
@@ -18662,7 +18662,7 @@
         <v>906</v>
       </c>
       <c r="R324" t="n">
-        <v>574</v>
+        <v>601</v>
       </c>
     </row>
     <row r="325">
@@ -18716,7 +18716,7 @@
         <v>80</v>
       </c>
       <c r="R325" t="n">
-        <v>20</v>
+        <v>110</v>
       </c>
     </row>
     <row r="326">
@@ -18770,7 +18770,7 @@
         <v>752</v>
       </c>
       <c r="R326" t="n">
-        <v>675</v>
+        <v>855</v>
       </c>
     </row>
     <row r="327">
@@ -18824,7 +18824,7 @@
         <v>98.125</v>
       </c>
       <c r="R327" t="n">
-        <v>21</v>
+        <v>98</v>
       </c>
     </row>
     <row r="328">
@@ -18878,7 +18878,7 @@
         <v>6948</v>
       </c>
       <c r="R328" t="n">
-        <v>2666</v>
+        <v>6280</v>
       </c>
     </row>
     <row r="329">
@@ -18932,7 +18932,7 @@
         <v>1426</v>
       </c>
       <c r="R329" t="n">
-        <v>995</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="330">
@@ -18986,7 +18986,7 @@
         <v>104.875</v>
       </c>
       <c r="R330" t="n">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="331">
@@ -19040,7 +19040,7 @@
         <v>29.40625</v>
       </c>
       <c r="R331" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="332">
@@ -19094,7 +19094,7 @@
         <v>759</v>
       </c>
       <c r="R332" t="n">
-        <v>580</v>
+        <v>588</v>
       </c>
     </row>
     <row r="333">
@@ -19148,7 +19148,7 @@
         <v>116.125</v>
       </c>
       <c r="R333" t="n">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
     <row r="334">
@@ -19200,7 +19200,7 @@
       </c>
       <c r="Q334" t="inlineStr"/>
       <c r="R334" t="n">
-        <v>424</v>
+        <v>536</v>
       </c>
     </row>
     <row r="335">
@@ -19248,7 +19248,7 @@
       <c r="P335" t="inlineStr"/>
       <c r="Q335" t="inlineStr"/>
       <c r="R335" t="n">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="336">
@@ -19302,7 +19302,7 @@
         <v>22.796875</v>
       </c>
       <c r="R336" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="337">
@@ -19356,7 +19356,7 @@
         <v>157.5</v>
       </c>
       <c r="R337" t="n">
-        <v>133</v>
+        <v>165</v>
       </c>
     </row>
     <row r="338">
@@ -19462,7 +19462,7 @@
         <v>46.78125</v>
       </c>
       <c r="R339" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="340">
@@ -19516,7 +19516,7 @@
         <v>265.5</v>
       </c>
       <c r="R340" t="n">
-        <v>58</v>
+        <v>166</v>
       </c>
     </row>
     <row r="341">
@@ -19570,7 +19570,7 @@
         <v>54</v>
       </c>
       <c r="R341" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="342">
@@ -19624,7 +19624,7 @@
         <v>1782</v>
       </c>
       <c r="R342" t="n">
-        <v>877</v>
+        <v>967</v>
       </c>
     </row>
     <row r="343">
@@ -19678,7 +19678,7 @@
         <v>332.5</v>
       </c>
       <c r="R343" t="n">
-        <v>149</v>
+        <v>224</v>
       </c>
     </row>
     <row r="344">
@@ -19732,7 +19732,7 @@
         <v>64.5</v>
       </c>
       <c r="R344" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="345">
@@ -19786,7 +19786,7 @@
         <v>571</v>
       </c>
       <c r="R345" t="n">
-        <v>529</v>
+        <v>514</v>
       </c>
     </row>
     <row r="346">
@@ -19840,7 +19840,7 @@
         <v>45.5</v>
       </c>
       <c r="R346" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="347">
@@ -19894,7 +19894,7 @@
         <v>785</v>
       </c>
       <c r="R347" t="n">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="348">
@@ -19948,7 +19948,7 @@
         <v>75</v>
       </c>
       <c r="R348" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="349">
@@ -19996,7 +19996,7 @@
       <c r="P349" t="inlineStr"/>
       <c r="Q349" t="inlineStr"/>
       <c r="R349" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="350">
@@ -20050,7 +20050,7 @@
         <v>977.5</v>
       </c>
       <c r="R350" t="n">
-        <v>662</v>
+        <v>862</v>
       </c>
     </row>
     <row r="351">
@@ -20104,7 +20104,7 @@
         <v>37.5</v>
       </c>
       <c r="R351" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="352">
@@ -20158,7 +20158,7 @@
         <v>7868</v>
       </c>
       <c r="R352" t="n">
-        <v>2571</v>
+        <v>6947</v>
       </c>
     </row>
     <row r="353">
@@ -20212,7 +20212,7 @@
         <v>357.5</v>
       </c>
       <c r="R353" t="n">
-        <v>247</v>
+        <v>340</v>
       </c>
     </row>
     <row r="354">
@@ -20266,7 +20266,7 @@
         <v>296.5</v>
       </c>
       <c r="R354" t="n">
-        <v>114</v>
+        <v>240</v>
       </c>
     </row>
     <row r="355">
@@ -20320,7 +20320,7 @@
         <v>132.5</v>
       </c>
       <c r="R355" t="n">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="356">
@@ -20374,7 +20374,7 @@
         <v>139.5</v>
       </c>
       <c r="R356" t="n">
-        <v>42</v>
+        <v>140</v>
       </c>
     </row>
     <row r="357">
@@ -20428,7 +20428,7 @@
         <v>56.40625</v>
       </c>
       <c r="R357" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="358">
@@ -20482,7 +20482,7 @@
         <v>37.0625</v>
       </c>
       <c r="R358" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="359">
@@ -20536,7 +20536,7 @@
         <v>23.84375</v>
       </c>
       <c r="R359" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="360">
@@ -20590,7 +20590,7 @@
         <v>23.09375</v>
       </c>
       <c r="R360" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="361">
@@ -20640,7 +20640,7 @@
       <c r="P361" t="inlineStr"/>
       <c r="Q361" t="inlineStr"/>
       <c r="R361" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="362">
@@ -20694,7 +20694,7 @@
         <v>172.75</v>
       </c>
       <c r="R362" t="n">
-        <v>65</v>
+        <v>187</v>
       </c>
     </row>
     <row r="363">
@@ -20748,7 +20748,7 @@
         <v>52.5</v>
       </c>
       <c r="R363" t="n">
-        <v>10</v>
+        <v>86</v>
       </c>
     </row>
     <row r="364">
@@ -20802,7 +20802,7 @@
         <v>1210</v>
       </c>
       <c r="R364" t="n">
-        <v>1361</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="365">
@@ -20856,7 +20856,7 @@
         <v>807.5</v>
       </c>
       <c r="R365" t="n">
-        <v>608</v>
+        <v>697</v>
       </c>
     </row>
     <row r="366">
@@ -20910,7 +20910,7 @@
         <v>550</v>
       </c>
       <c r="R366" t="n">
-        <v>589</v>
+        <v>661</v>
       </c>
     </row>
     <row r="367">
@@ -20964,7 +20964,7 @@
         <v>300.5</v>
       </c>
       <c r="R367" t="n">
-        <v>225</v>
+        <v>353</v>
       </c>
     </row>
     <row r="368">
@@ -21018,7 +21018,7 @@
         <v>51.5625</v>
       </c>
       <c r="R368" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="369">
@@ -21072,7 +21072,7 @@
         <v>267.5</v>
       </c>
       <c r="R369" t="n">
-        <v>156</v>
+        <v>223</v>
       </c>
     </row>
     <row r="370">
@@ -21124,7 +21124,7 @@
         <v>17.4375</v>
       </c>
       <c r="R370" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="371">
@@ -21178,7 +21178,7 @@
         <v>257.5</v>
       </c>
       <c r="R371" t="n">
-        <v>100</v>
+        <v>209</v>
       </c>
     </row>
     <row r="372">
@@ -21232,7 +21232,7 @@
         <v>789.5</v>
       </c>
       <c r="R372" t="n">
-        <v>601</v>
+        <v>624</v>
       </c>
     </row>
     <row r="373">
@@ -21284,7 +21284,7 @@
         <v>590</v>
       </c>
       <c r="R373" t="n">
-        <v>296</v>
+        <v>573</v>
       </c>
     </row>
     <row r="374">
@@ -21338,7 +21338,7 @@
         <v>2878</v>
       </c>
       <c r="R374" t="n">
-        <v>1318</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="375">
@@ -21392,7 +21392,7 @@
         <v>360</v>
       </c>
       <c r="R375" t="n">
-        <v>358</v>
+        <v>542</v>
       </c>
     </row>
     <row r="376">
@@ -21446,7 +21446,7 @@
         <v>658.5</v>
       </c>
       <c r="R376" t="n">
-        <v>658</v>
+        <v>765</v>
       </c>
     </row>
     <row r="377">
@@ -21500,7 +21500,7 @@
         <v>103.5</v>
       </c>
       <c r="R377" t="n">
-        <v>22</v>
+        <v>95</v>
       </c>
     </row>
     <row r="378">
@@ -21554,7 +21554,7 @@
         <v>3202</v>
       </c>
       <c r="R378" t="n">
-        <v>1383</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="379">
@@ -21608,7 +21608,7 @@
         <v>458</v>
       </c>
       <c r="R379" t="n">
-        <v>552</v>
+        <v>631</v>
       </c>
     </row>
     <row r="380">
@@ -21662,7 +21662,7 @@
         <v>8888</v>
       </c>
       <c r="R380" t="n">
-        <v>2851</v>
+        <v>8956</v>
       </c>
     </row>
     <row r="381">
@@ -21716,7 +21716,7 @@
         <v>1151</v>
       </c>
       <c r="R381" t="n">
-        <v>981</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="382">
@@ -21770,7 +21770,7 @@
         <v>113.6875</v>
       </c>
       <c r="R382" t="n">
-        <v>30</v>
+        <v>94</v>
       </c>
     </row>
     <row r="383">
@@ -21824,7 +21824,7 @@
         <v>311</v>
       </c>
       <c r="R383" t="n">
-        <v>228</v>
+        <v>293</v>
       </c>
     </row>
     <row r="384">
@@ -21872,7 +21872,7 @@
       <c r="P384" t="inlineStr"/>
       <c r="Q384" t="inlineStr"/>
       <c r="R384" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="385">
@@ -21926,7 +21926,7 @@
         <v>319</v>
       </c>
       <c r="R385" t="n">
-        <v>356</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386">
@@ -21980,7 +21980,7 @@
         <v>2332</v>
       </c>
       <c r="R386" t="n">
-        <v>1423</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="387">
@@ -22034,7 +22034,7 @@
         <v>294.25</v>
       </c>
       <c r="R387" t="n">
-        <v>98</v>
+        <v>274</v>
       </c>
     </row>
     <row r="388">
@@ -22088,7 +22088,7 @@
         <v>125.6875</v>
       </c>
       <c r="R388" t="n">
-        <v>16</v>
+        <v>62</v>
       </c>
     </row>
     <row r="389">
@@ -22142,7 +22142,7 @@
         <v>21.296875</v>
       </c>
       <c r="R389" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="390">
@@ -22196,7 +22196,7 @@
         <v>932</v>
       </c>
       <c r="R390" t="n">
-        <v>606</v>
+        <v>739</v>
       </c>
     </row>
     <row r="391">
@@ -22250,7 +22250,7 @@
         <v>1316</v>
       </c>
       <c r="R391" t="n">
-        <v>640</v>
+        <v>798</v>
       </c>
     </row>
     <row r="392">
@@ -22304,7 +22304,7 @@
         <v>125</v>
       </c>
       <c r="R392" t="n">
-        <v>13</v>
+        <v>84</v>
       </c>
     </row>
     <row r="393">
@@ -22358,7 +22358,7 @@
         <v>737</v>
       </c>
       <c r="R393" t="n">
-        <v>595</v>
+        <v>623</v>
       </c>
     </row>
     <row r="394">
@@ -22412,7 +22412,7 @@
         <v>141.625</v>
       </c>
       <c r="R394" t="n">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="395">
@@ -22466,7 +22466,7 @@
         <v>6760</v>
       </c>
       <c r="R395" t="n">
-        <v>2302</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="396">
@@ -22520,7 +22520,7 @@
         <v>911</v>
       </c>
       <c r="R396" t="n">
-        <v>640</v>
+        <v>753</v>
       </c>
     </row>
     <row r="397">
@@ -22574,7 +22574,7 @@
         <v>255.25</v>
       </c>
       <c r="R397" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="398">
@@ -22628,7 +22628,7 @@
         <v>37.5</v>
       </c>
       <c r="R398" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="399">
@@ -22682,7 +22682,7 @@
         <v>764</v>
       </c>
       <c r="R399" t="n">
-        <v>270</v>
+        <v>474</v>
       </c>
     </row>
     <row r="400">
@@ -22736,7 +22736,7 @@
         <v>249</v>
       </c>
       <c r="R400" t="n">
-        <v>44</v>
+        <v>116</v>
       </c>
     </row>
     <row r="401">
@@ -22784,7 +22784,7 @@
       <c r="P401" t="inlineStr"/>
       <c r="Q401" t="inlineStr"/>
       <c r="R401" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="402">
@@ -22838,7 +22838,7 @@
         <v>93.625</v>
       </c>
       <c r="R402" t="n">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="403">
@@ -22892,7 +22892,7 @@
         <v>1196</v>
       </c>
       <c r="R403" t="n">
-        <v>700</v>
+        <v>871</v>
       </c>
     </row>
     <row r="404">
@@ -22946,7 +22946,7 @@
         <v>114.625</v>
       </c>
       <c r="R404" t="n">
-        <v>9</v>
+        <v>108</v>
       </c>
     </row>
     <row r="405">
@@ -23000,7 +23000,7 @@
         <v>896</v>
       </c>
       <c r="R405" t="n">
-        <v>628</v>
+        <v>684</v>
       </c>
     </row>
     <row r="406">
@@ -23054,7 +23054,7 @@
         <v>49.8125</v>
       </c>
       <c r="R406" t="n">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="407">
@@ -23106,7 +23106,7 @@
       </c>
       <c r="Q407" t="inlineStr"/>
       <c r="R407" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="408">
@@ -23160,7 +23160,7 @@
         <v>31.5</v>
       </c>
       <c r="R408" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="409">
@@ -23214,7 +23214,7 @@
         <v>1199</v>
       </c>
       <c r="R409" t="n">
-        <v>673</v>
+        <v>813</v>
       </c>
     </row>
     <row r="410">
@@ -23268,7 +23268,7 @@
         <v>20</v>
       </c>
       <c r="R410" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="411">
@@ -23322,7 +23322,7 @@
         <v>198.125</v>
       </c>
       <c r="R411" t="n">
-        <v>254</v>
+        <v>401</v>
       </c>
     </row>
     <row r="412">
@@ -23370,7 +23370,7 @@
       <c r="P412" t="inlineStr"/>
       <c r="Q412" t="inlineStr"/>
       <c r="R412" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="413">
@@ -23424,7 +23424,7 @@
         <v>594</v>
       </c>
       <c r="R413" t="n">
-        <v>632</v>
+        <v>747</v>
       </c>
     </row>
     <row r="414">
@@ -23478,7 +23478,7 @@
         <v>46.1875</v>
       </c>
       <c r="R414" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
     </row>
     <row r="415">
@@ -23532,7 +23532,7 @@
         <v>4656</v>
       </c>
       <c r="R415" t="n">
-        <v>1852</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="416">
@@ -23586,7 +23586,7 @@
         <v>437.5</v>
       </c>
       <c r="R416" t="n">
-        <v>529</v>
+        <v>588</v>
       </c>
     </row>
     <row r="417">
@@ -23640,7 +23640,7 @@
         <v>751</v>
       </c>
       <c r="R417" t="n">
-        <v>560</v>
+        <v>589</v>
       </c>
     </row>
     <row r="418">
@@ -23694,7 +23694,7 @@
         <v>95</v>
       </c>
       <c r="R418" t="n">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="419">
@@ -23748,7 +23748,7 @@
         <v>591.5</v>
       </c>
       <c r="R419" t="n">
-        <v>651</v>
+        <v>862</v>
       </c>
     </row>
     <row r="420">
@@ -23802,7 +23802,7 @@
         <v>69.625</v>
       </c>
       <c r="R420" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="421">
@@ -23856,7 +23856,7 @@
         <v>6168</v>
       </c>
       <c r="R421" t="n">
-        <v>2559</v>
+        <v>6148</v>
       </c>
     </row>
     <row r="422">
@@ -23910,7 +23910,7 @@
         <v>1390</v>
       </c>
       <c r="R422" t="n">
-        <v>1001</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="423">
@@ -23964,7 +23964,7 @@
         <v>87.625</v>
       </c>
       <c r="R423" t="n">
-        <v>23</v>
+        <v>69</v>
       </c>
     </row>
     <row r="424">
@@ -24018,7 +24018,7 @@
         <v>22.65625</v>
       </c>
       <c r="R424" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="425">
@@ -24072,7 +24072,7 @@
         <v>635</v>
       </c>
       <c r="R425" t="n">
-        <v>567</v>
+        <v>594</v>
       </c>
     </row>
     <row r="426">
@@ -24126,7 +24126,7 @@
         <v>71.125</v>
       </c>
       <c r="R426" t="n">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="427">
@@ -24178,7 +24178,7 @@
       </c>
       <c r="Q427" t="inlineStr"/>
       <c r="R427" t="n">
-        <v>421</v>
+        <v>537</v>
       </c>
     </row>
     <row r="428">
@@ -24226,7 +24226,7 @@
       <c r="P428" t="inlineStr"/>
       <c r="Q428" t="inlineStr"/>
       <c r="R428" t="n">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="429">
@@ -24280,7 +24280,7 @@
         <v>18</v>
       </c>
       <c r="R429" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="430">
@@ -24334,7 +24334,7 @@
         <v>163.5</v>
       </c>
       <c r="R430" t="n">
-        <v>141</v>
+        <v>169</v>
       </c>
     </row>
     <row r="431">
@@ -24440,7 +24440,7 @@
         <v>75.25</v>
       </c>
       <c r="R432" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="433">
@@ -24494,7 +24494,7 @@
         <v>260</v>
       </c>
       <c r="R433" t="n">
-        <v>57</v>
+        <v>158</v>
       </c>
     </row>
     <row r="434">
@@ -24548,7 +24548,7 @@
         <v>31.796875</v>
       </c>
       <c r="R434" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="435">
@@ -24602,7 +24602,7 @@
         <v>1404</v>
       </c>
       <c r="R435" t="n">
-        <v>869</v>
+        <v>904</v>
       </c>
     </row>
     <row r="436">
@@ -24656,7 +24656,7 @@
         <v>248</v>
       </c>
       <c r="R436" t="n">
-        <v>149</v>
+        <v>194</v>
       </c>
     </row>
     <row r="437">
@@ -24710,7 +24710,7 @@
         <v>51.59375</v>
       </c>
       <c r="R437" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="438">
@@ -24764,7 +24764,7 @@
         <v>583</v>
       </c>
       <c r="R438" t="n">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="439">
@@ -24818,7 +24818,7 @@
         <v>37.5</v>
       </c>
       <c r="R439" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="440">
@@ -24872,7 +24872,7 @@
         <v>677</v>
       </c>
       <c r="R440" t="n">
-        <v>589</v>
+        <v>604</v>
       </c>
     </row>
     <row r="441">
@@ -24926,7 +24926,7 @@
         <v>55</v>
       </c>
       <c r="R441" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="442">
@@ -24974,7 +24974,7 @@
       <c r="P442" t="inlineStr"/>
       <c r="Q442" t="inlineStr"/>
       <c r="R442" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="443">
@@ -25028,7 +25028,7 @@
         <v>829</v>
       </c>
       <c r="R443" t="n">
-        <v>644</v>
+        <v>862</v>
       </c>
     </row>
     <row r="444">
@@ -25082,7 +25082,7 @@
         <v>26.703125</v>
       </c>
       <c r="R444" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="445">
@@ -25136,7 +25136,7 @@
         <v>7272</v>
       </c>
       <c r="R445" t="n">
-        <v>2469</v>
+        <v>7330</v>
       </c>
     </row>
     <row r="446">
@@ -25190,7 +25190,7 @@
         <v>269</v>
       </c>
       <c r="R446" t="n">
-        <v>244</v>
+        <v>289</v>
       </c>
     </row>
     <row r="447">
@@ -25244,7 +25244,7 @@
         <v>309</v>
       </c>
       <c r="R447" t="n">
-        <v>122</v>
+        <v>206</v>
       </c>
     </row>
     <row r="448">
@@ -25298,7 +25298,7 @@
         <v>57.5</v>
       </c>
       <c r="R448" t="n">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="449">
@@ -25352,7 +25352,7 @@
         <v>172</v>
       </c>
       <c r="R449" t="n">
-        <v>41</v>
+        <v>117</v>
       </c>
     </row>
     <row r="450">
@@ -25406,7 +25406,7 @@
         <v>44.6875</v>
       </c>
       <c r="R450" t="n">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="451">
@@ -25460,7 +25460,7 @@
         <v>32.84375</v>
       </c>
       <c r="R451" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="452">
@@ -25514,7 +25514,7 @@
         <v>24</v>
       </c>
       <c r="R452" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="453">
@@ -25568,7 +25568,7 @@
         <v>21</v>
       </c>
       <c r="R453" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="454">
@@ -25618,7 +25618,7 @@
       <c r="P454" t="inlineStr"/>
       <c r="Q454" t="inlineStr"/>
       <c r="R454" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="455">
@@ -25672,7 +25672,7 @@
         <v>77.5625</v>
       </c>
       <c r="R455" t="n">
-        <v>63</v>
+        <v>200</v>
       </c>
     </row>
     <row r="456">
@@ -25726,7 +25726,7 @@
         <v>41.25</v>
       </c>
       <c r="R456" t="n">
-        <v>12</v>
+        <v>76</v>
       </c>
     </row>
     <row r="457">
@@ -25780,7 +25780,7 @@
         <v>965</v>
       </c>
       <c r="R457" t="n">
-        <v>1427</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="458">
@@ -25834,7 +25834,7 @@
         <v>575</v>
       </c>
       <c r="R458" t="n">
-        <v>563</v>
+        <v>595</v>
       </c>
     </row>
     <row r="459">
@@ -25888,7 +25888,7 @@
         <v>408.5</v>
       </c>
       <c r="R459" t="n">
-        <v>586</v>
+        <v>697</v>
       </c>
     </row>
     <row r="460">
@@ -25942,7 +25942,7 @@
         <v>281.5</v>
       </c>
       <c r="R460" t="n">
-        <v>228</v>
+        <v>279</v>
       </c>
     </row>
     <row r="461">
@@ -25996,7 +25996,7 @@
         <v>45.59375</v>
       </c>
       <c r="R461" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="462">
@@ -26050,7 +26050,7 @@
         <v>404</v>
       </c>
       <c r="R462" t="n">
-        <v>166</v>
+        <v>207</v>
       </c>
     </row>
     <row r="463">
@@ -26102,7 +26102,7 @@
         <v>50.5</v>
       </c>
       <c r="R463" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="464">
@@ -26156,7 +26156,7 @@
         <v>226.5</v>
       </c>
       <c r="R464" t="n">
-        <v>102</v>
+        <v>208</v>
       </c>
     </row>
     <row r="465">
@@ -26210,7 +26210,7 @@
         <v>573.5</v>
       </c>
       <c r="R465" t="n">
-        <v>575</v>
+        <v>612</v>
       </c>
     </row>
     <row r="466">
@@ -26262,7 +26262,7 @@
         <v>528</v>
       </c>
       <c r="R466" t="n">
-        <v>287</v>
+        <v>495</v>
       </c>
     </row>
     <row r="467">
@@ -26316,7 +26316,7 @@
         <v>3026</v>
       </c>
       <c r="R467" t="n">
-        <v>1297</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="468">
@@ -26370,7 +26370,7 @@
         <v>420</v>
       </c>
       <c r="R468" t="n">
-        <v>419</v>
+        <v>595</v>
       </c>
     </row>
     <row r="469">
@@ -26424,7 +26424,7 @@
         <v>814</v>
       </c>
       <c r="R469" t="n">
-        <v>690</v>
+        <v>827</v>
       </c>
     </row>
     <row r="470">
@@ -26478,7 +26478,7 @@
         <v>108.875</v>
       </c>
       <c r="R470" t="n">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="471">
@@ -26532,7 +26532,7 @@
         <v>3372</v>
       </c>
       <c r="R471" t="n">
-        <v>1404</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="472">
@@ -26586,7 +26586,7 @@
         <v>609</v>
       </c>
       <c r="R472" t="n">
-        <v>601</v>
+        <v>706</v>
       </c>
     </row>
     <row r="473">
@@ -26640,7 +26640,7 @@
         <v>10848</v>
       </c>
       <c r="R473" t="n">
-        <v>3171</v>
+        <v>10793</v>
       </c>
     </row>
     <row r="474">
@@ -26694,7 +26694,7 @@
         <v>1548</v>
       </c>
       <c r="R474" t="n">
-        <v>999</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="475">
@@ -26748,7 +26748,7 @@
         <v>134.75</v>
       </c>
       <c r="R475" t="n">
-        <v>32</v>
+        <v>105</v>
       </c>
     </row>
     <row r="476">
@@ -26802,7 +26802,7 @@
         <v>395.5</v>
       </c>
       <c r="R476" t="n">
-        <v>253</v>
+        <v>337</v>
       </c>
     </row>
     <row r="477">
@@ -26850,7 +26850,7 @@
       <c r="P477" t="inlineStr"/>
       <c r="Q477" t="inlineStr"/>
       <c r="R477" t="n">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="478">
@@ -26904,7 +26904,7 @@
         <v>336.5</v>
       </c>
       <c r="R478" t="n">
-        <v>382</v>
+        <v>451</v>
       </c>
     </row>
     <row r="479">
@@ -26958,7 +26958,7 @@
         <v>2530</v>
       </c>
       <c r="R479" t="n">
-        <v>1451</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="480">
@@ -27012,7 +27012,7 @@
         <v>365.5</v>
       </c>
       <c r="R480" t="n">
-        <v>103</v>
+        <v>246</v>
       </c>
     </row>
     <row r="481">
@@ -27066,7 +27066,7 @@
         <v>137.75</v>
       </c>
       <c r="R481" t="n">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="482">
@@ -27120,7 +27120,7 @@
         <v>39.90625</v>
       </c>
       <c r="R482" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="483">
@@ -27174,7 +27174,7 @@
         <v>1026</v>
       </c>
       <c r="R483" t="n">
-        <v>626</v>
+        <v>753</v>
       </c>
     </row>
     <row r="484">
@@ -27228,7 +27228,7 @@
         <v>1209</v>
       </c>
       <c r="R484" t="n">
-        <v>651</v>
+        <v>792</v>
       </c>
     </row>
     <row r="485">
@@ -27282,7 +27282,7 @@
         <v>170</v>
       </c>
       <c r="R485" t="n">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="486">
@@ -27336,7 +27336,7 @@
         <v>728</v>
       </c>
       <c r="R486" t="n">
-        <v>612</v>
+        <v>663</v>
       </c>
     </row>
     <row r="487">
@@ -27390,7 +27390,7 @@
         <v>148.75</v>
       </c>
       <c r="R487" t="n">
-        <v>38</v>
+        <v>117</v>
       </c>
     </row>
     <row r="488">
@@ -27444,7 +27444,7 @@
         <v>7508</v>
       </c>
       <c r="R488" t="n">
-        <v>2320</v>
+        <v>6196</v>
       </c>
     </row>
     <row r="489">
@@ -27498,7 +27498,7 @@
         <v>1147</v>
       </c>
       <c r="R489" t="n">
-        <v>687</v>
+        <v>886</v>
       </c>
     </row>
     <row r="490">
@@ -27552,7 +27552,7 @@
         <v>233.375</v>
       </c>
       <c r="R490" t="n">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="491">
@@ -27606,7 +27606,7 @@
         <v>86.125</v>
       </c>
       <c r="R491" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="492">
@@ -27660,7 +27660,7 @@
         <v>812</v>
       </c>
       <c r="R492" t="n">
-        <v>269</v>
+        <v>463</v>
       </c>
     </row>
     <row r="493">
@@ -27714,7 +27714,7 @@
         <v>209.625</v>
       </c>
       <c r="R493" t="n">
-        <v>47</v>
+        <v>141</v>
       </c>
     </row>
     <row r="494">
@@ -27762,7 +27762,7 @@
       <c r="P494" t="inlineStr"/>
       <c r="Q494" t="inlineStr"/>
       <c r="R494" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="495">
@@ -27816,7 +27816,7 @@
         <v>109.8125</v>
       </c>
       <c r="R495" t="n">
-        <v>21</v>
+        <v>80</v>
       </c>
     </row>
     <row r="496">
@@ -27870,7 +27870,7 @@
         <v>1136</v>
       </c>
       <c r="R496" t="n">
-        <v>721</v>
+        <v>908</v>
       </c>
     </row>
     <row r="497">
@@ -27924,7 +27924,7 @@
         <v>142.75</v>
       </c>
       <c r="R497" t="n">
-        <v>14</v>
+        <v>110</v>
       </c>
     </row>
     <row r="498">
@@ -27978,7 +27978,7 @@
         <v>897</v>
       </c>
       <c r="R498" t="n">
-        <v>650</v>
+        <v>720</v>
       </c>
     </row>
     <row r="499">
@@ -28032,7 +28032,7 @@
         <v>56.09375</v>
       </c>
       <c r="R499" t="n">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="500">
@@ -28084,7 +28084,7 @@
       </c>
       <c r="Q500" t="inlineStr"/>
       <c r="R500" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="501">
@@ -28136,7 +28136,7 @@
         <v>23.40625</v>
       </c>
       <c r="R501" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="502">
@@ -28190,7 +28190,7 @@
         <v>1029</v>
       </c>
       <c r="R502" t="n">
-        <v>686</v>
+        <v>857</v>
       </c>
     </row>
     <row r="503">
@@ -28244,7 +28244,7 @@
         <v>10</v>
       </c>
       <c r="R503" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="504">
@@ -28298,7 +28298,7 @@
         <v>274.25</v>
       </c>
       <c r="R504" t="n">
-        <v>283</v>
+        <v>426</v>
       </c>
     </row>
     <row r="505">
@@ -28346,7 +28346,7 @@
       <c r="P505" t="inlineStr"/>
       <c r="Q505" t="inlineStr"/>
       <c r="R505" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="506">
@@ -28400,7 +28400,7 @@
         <v>715</v>
       </c>
       <c r="R506" t="n">
-        <v>646</v>
+        <v>746</v>
       </c>
     </row>
     <row r="507">
@@ -28454,7 +28454,7 @@
         <v>62.6875</v>
       </c>
       <c r="R507" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="508">
@@ -28508,7 +28508,7 @@
         <v>5400</v>
       </c>
       <c r="R508" t="n">
-        <v>1881</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="509">
@@ -28562,7 +28562,7 @@
         <v>487.5</v>
       </c>
       <c r="R509" t="n">
-        <v>557</v>
+        <v>623</v>
       </c>
     </row>
     <row r="510">
@@ -28616,7 +28616,7 @@
         <v>485.5</v>
       </c>
       <c r="R510" t="n">
-        <v>545</v>
+        <v>554</v>
       </c>
     </row>
     <row r="511">
@@ -28670,7 +28670,7 @@
         <v>105</v>
       </c>
       <c r="R511" t="n">
-        <v>25</v>
+        <v>106</v>
       </c>
     </row>
     <row r="512">
@@ -28724,7 +28724,7 @@
         <v>791</v>
       </c>
       <c r="R512" t="n">
-        <v>645</v>
+        <v>761</v>
       </c>
     </row>
     <row r="513">
@@ -28778,7 +28778,7 @@
         <v>99.875</v>
       </c>
       <c r="R513" t="n">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="514">
@@ -28832,7 +28832,7 @@
         <v>7360</v>
       </c>
       <c r="R514" t="n">
-        <v>2571</v>
+        <v>6446</v>
       </c>
     </row>
     <row r="515">
@@ -28886,7 +28886,7 @@
         <v>1618</v>
       </c>
       <c r="R515" t="n">
-        <v>1026</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="516">
@@ -28940,7 +28940,7 @@
         <v>91.5</v>
       </c>
       <c r="R516" t="n">
-        <v>28</v>
+        <v>76</v>
       </c>
     </row>
     <row r="517">
@@ -28994,7 +28994,7 @@
         <v>24.75</v>
       </c>
       <c r="R517" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="518">
@@ -29048,7 +29048,7 @@
         <v>724.5</v>
       </c>
       <c r="R518" t="n">
-        <v>603</v>
+        <v>638</v>
       </c>
     </row>
     <row r="519">
@@ -29102,7 +29102,7 @@
         <v>86.125</v>
       </c>
       <c r="R519" t="n">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="520">
@@ -29154,7 +29154,7 @@
       </c>
       <c r="Q520" t="inlineStr"/>
       <c r="R520" t="n">
-        <v>453</v>
+        <v>565</v>
       </c>
     </row>
     <row r="521">
@@ -29202,7 +29202,7 @@
       <c r="P521" t="inlineStr"/>
       <c r="Q521" t="inlineStr"/>
       <c r="R521" t="n">
-        <v>56</v>
+        <v>85</v>
       </c>
     </row>
     <row r="522">
@@ -29256,7 +29256,7 @@
         <v>32.6875</v>
       </c>
       <c r="R522" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="523">
@@ -29310,7 +29310,7 @@
         <v>166</v>
       </c>
       <c r="R523" t="n">
-        <v>149</v>
+        <v>192</v>
       </c>
     </row>
     <row r="524">
@@ -29362,7 +29362,7 @@
         <v>7</v>
       </c>
       <c r="R524" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="525">
@@ -29416,7 +29416,7 @@
         <v>47.09375</v>
       </c>
       <c r="R525" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="526">
@@ -29470,7 +29470,7 @@
         <v>298.75</v>
       </c>
       <c r="R526" t="n">
-        <v>61</v>
+        <v>168</v>
       </c>
     </row>
     <row r="527">
@@ -29524,7 +29524,7 @@
         <v>63.90625</v>
       </c>
       <c r="R527" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="528">
@@ -29578,7 +29578,7 @@
         <v>1914</v>
       </c>
       <c r="R528" t="n">
-        <v>874</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="529">
@@ -29632,7 +29632,7 @@
         <v>350.5</v>
       </c>
       <c r="R529" t="n">
-        <v>159</v>
+        <v>191</v>
       </c>
     </row>
     <row r="530">
@@ -29686,7 +29686,7 @@
         <v>67.0625</v>
       </c>
       <c r="R530" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="531">
@@ -29740,7 +29740,7 @@
         <v>662</v>
       </c>
       <c r="R531" t="n">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="532">
@@ -29794,7 +29794,7 @@
         <v>41.5</v>
       </c>
       <c r="R532" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="533">
@@ -29848,7 +29848,7 @@
         <v>857.5</v>
       </c>
       <c r="R533" t="n">
-        <v>626</v>
+        <v>674</v>
       </c>
     </row>
     <row r="534">
@@ -29902,7 +29902,7 @@
         <v>45</v>
       </c>
       <c r="R534" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="535">
@@ -29950,7 +29950,7 @@
       <c r="P535" t="inlineStr"/>
       <c r="Q535" t="inlineStr"/>
       <c r="R535" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="536">
@@ -30004,7 +30004,7 @@
         <v>1082</v>
       </c>
       <c r="R536" t="n">
-        <v>664</v>
+        <v>886</v>
       </c>
     </row>
     <row r="537">
@@ -30058,7 +30058,7 @@
         <v>33.59375</v>
       </c>
       <c r="R537" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="538">
@@ -30112,7 +30112,7 @@
         <v>9200</v>
       </c>
       <c r="R538" t="n">
-        <v>2542</v>
+        <v>7291</v>
       </c>
     </row>
     <row r="539">
@@ -30166,7 +30166,7 @@
         <v>372.5</v>
       </c>
       <c r="R539" t="n">
-        <v>273</v>
+        <v>343</v>
       </c>
     </row>
     <row r="540">
@@ -30220,7 +30220,7 @@
         <v>300.5</v>
       </c>
       <c r="R540" t="n">
-        <v>129</v>
+        <v>260</v>
       </c>
     </row>
     <row r="541">
@@ -30274,7 +30274,7 @@
         <v>116.5</v>
       </c>
       <c r="R541" t="n">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="542">
@@ -30328,7 +30328,7 @@
         <v>242.5</v>
       </c>
       <c r="R542" t="n">
-        <v>49</v>
+        <v>122</v>
       </c>
     </row>
     <row r="543">
@@ -30382,7 +30382,7 @@
         <v>59.40625</v>
       </c>
       <c r="R543" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="544">
@@ -30436,7 +30436,7 @@
         <v>42.3125</v>
       </c>
       <c r="R544" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="545">
@@ -30490,7 +30490,7 @@
         <v>31.046875</v>
       </c>
       <c r="R545" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="546">
@@ -30544,7 +30544,7 @@
         <v>20.546875</v>
       </c>
       <c r="R546" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="547">
@@ -30594,7 +30594,7 @@
       <c r="P547" t="inlineStr"/>
       <c r="Q547" t="inlineStr"/>
       <c r="R547" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="548">
@@ -30648,7 +30648,7 @@
         <v>108</v>
       </c>
       <c r="R548" t="n">
-        <v>66</v>
+        <v>192</v>
       </c>
     </row>
     <row r="549">
@@ -30702,7 +30702,7 @@
         <v>40.5</v>
       </c>
       <c r="R549" t="n">
-        <v>17</v>
+        <v>89</v>
       </c>
     </row>
     <row r="550">
@@ -30756,7 +30756,7 @@
         <v>1370</v>
       </c>
       <c r="R550" t="n">
-        <v>1480</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="551">
@@ -30810,7 +30810,7 @@
         <v>674.5</v>
       </c>
       <c r="R551" t="n">
-        <v>633</v>
+        <v>735</v>
       </c>
     </row>
     <row r="552">
@@ -30864,7 +30864,7 @@
         <v>562</v>
       </c>
       <c r="R552" t="n">
-        <v>659</v>
+        <v>794</v>
       </c>
     </row>
     <row r="553">
@@ -30918,7 +30918,7 @@
         <v>259.5</v>
       </c>
       <c r="R553" t="n">
-        <v>269</v>
+        <v>346</v>
       </c>
     </row>
     <row r="554">
@@ -30972,7 +30972,7 @@
         <v>54.625</v>
       </c>
       <c r="R554" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="555">
@@ -31026,7 +31026,7 @@
         <v>313.5</v>
       </c>
       <c r="R555" t="n">
-        <v>184</v>
+        <v>257</v>
       </c>
     </row>
     <row r="556">
@@ -31078,7 +31078,7 @@
         <v>13.3125</v>
       </c>
       <c r="R556" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="557">
@@ -31132,7 +31132,7 @@
         <v>277</v>
       </c>
       <c r="R557" t="n">
-        <v>120</v>
+        <v>240</v>
       </c>
     </row>
     <row r="558">
@@ -31186,7 +31186,7 @@
         <v>881.5</v>
       </c>
       <c r="R558" t="n">
-        <v>630</v>
+        <v>715</v>
       </c>
     </row>
     <row r="559">
@@ -31238,7 +31238,7 @@
         <v>653.5</v>
       </c>
       <c r="R559" t="n">
-        <v>313</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>